<commit_message>
🔧 Corregir manejo de resoluciones en carga masiva de vehículos
- ✅ Separar resolución primigenia (PADRE) y resolución hija (derivada)
- ✅ Actualizar validaciones para distinguir tipos de resolución
- ✅ Mejorar lógica de asignación de resoluciones en vehículos
- ✅ Actualizar plantilla Excel con nueva estructura
- ✅ Corregir pruebas y documentación
- ✅ Mantener compatibilidad con rutas existentes

Cambios técnicos:
- Modelo VehiculoExcel actualizado con campos específicos
- Validaciones mejoradas para tipos de resolución
- Lógica de priorización: resolución hija > primigenia
- Plantilla Excel actualizada con ejemplos correctos
- Todas las pruebas pasando exitosamente
</commit_message>
<xml_diff>
--- a/backend/plantilla_descargada.xlsx
+++ b/backend/plantilla_descargada.xlsx
@@ -446,12 +446,12 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Resolución Padre</t>
+          <t>Resolución Primigenia</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Resolución Primigenia</t>
+          <t>Resolución Hija</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -576,11 +576,7 @@
           <t>001-2024-DRTC-PUNO</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>001-2024-DRTC-PUNO</t>
-        </is>
-      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
           <t>01,02</t>
@@ -683,11 +679,7 @@
           <t>002-2024-DRTC-PUNO</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>002-2024-DRTC-PUNO</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
           <t>03</t>

</xml_diff>